<commit_message>
Added all states to dataset.
</commit_message>
<xml_diff>
--- a/data-v1.xlsx
+++ b/data-v1.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">N/A </t>
   </si>
   <si>
-    <t>Indiana</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -120,6 +117,153 @@
   </si>
   <si>
     <t>% other</t>
+  </si>
+  <si>
+    <t>ALASKA</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>IOWA</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>MONTANA</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>NEW JERSEY</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>VERMONT</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
   </si>
 </sst>
 </file>
@@ -438,17 +582,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="A17" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
@@ -462,8 +606,8 @@
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="9.85546875" customWidth="1"/>
     <col min="22" max="22" width="10.7109375" customWidth="1"/>
@@ -479,238 +623,443 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>22</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D2">
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E14" s="1">
         <v>0.245</v>
       </c>
-      <c r="F2">
+      <c r="F14">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G14" s="1">
         <v>9.4E-2</v>
       </c>
-      <c r="H2">
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I14" s="1">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J2">
+      <c r="J14">
         <v>53</v>
       </c>
-      <c r="K2">
+      <c r="K14">
         <v>12</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L14" s="1">
         <v>0.92300000000000004</v>
       </c>
-      <c r="M2">
+      <c r="M14">
         <v>3</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N14" t="s">
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="O14">
         <v>7</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P14" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="Q2">
+      <c r="Q14">
         <v>6</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R14" s="1">
         <v>0.46200000000000002</v>
       </c>
-      <c r="S2">
+      <c r="S14">
         <v>10</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T14" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="U2">
+      <c r="U14">
         <v>22</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V14" s="1">
         <v>0.68799999999999994</v>
       </c>
-      <c r="W2">
+      <c r="W14">
         <v>11</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X14" s="1">
         <v>0.34399999999999997</v>
       </c>
-      <c r="Y2">
+      <c r="Y14">
         <v>31</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z14" s="1">
         <v>0.96899999999999997</v>
       </c>
-      <c r="AA2">
+      <c r="AA14">
         <v>0</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB14" s="1">
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AC14">
         <v>16</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD14" s="1">
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-    </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a second option for what our dataset could look like. No percentages.
</commit_message>
<xml_diff>
--- a/data-v1.xlsx
+++ b/data-v1.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
-  <si>
-    <t xml:space="preserve">N/A </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>state</t>
   </si>
@@ -41,82 +38,43 @@
     <t># minors labor</t>
   </si>
   <si>
-    <t>% adult labor</t>
-  </si>
-  <si>
     <t># males labor</t>
   </si>
   <si>
-    <t>% females labor</t>
-  </si>
-  <si>
     <t># females labor</t>
   </si>
   <si>
-    <t>% males labor</t>
-  </si>
-  <si>
     <t># other</t>
   </si>
   <si>
     <t># other labor</t>
   </si>
   <si>
-    <t>% other labor</t>
-  </si>
-  <si>
-    <t>% minors labor</t>
-  </si>
-  <si>
-    <t>% adult sex</t>
-  </si>
-  <si>
     <t># minors sex</t>
   </si>
   <si>
-    <t>% minors sex</t>
-  </si>
-  <si>
     <t># females sex</t>
   </si>
   <si>
-    <t>% females sex</t>
-  </si>
-  <si>
     <t># males sex</t>
   </si>
   <si>
-    <t>% males sex</t>
-  </si>
-  <si>
     <t># other sex</t>
   </si>
   <si>
-    <t>% other sex</t>
-  </si>
-  <si>
     <t># adult sex</t>
   </si>
   <si>
     <t># sex</t>
   </si>
   <si>
-    <t>% sex</t>
-  </si>
-  <si>
     <t># labor</t>
   </si>
   <si>
-    <t>% labor</t>
-  </si>
-  <si>
     <t># sex &amp; labor</t>
   </si>
   <si>
-    <t>% sex &amp; labor</t>
-  </si>
-  <si>
-    <t>% other</t>
+    <t>ALABAMA</t>
   </si>
   <si>
     <t>ALASKA</t>
@@ -264,6 +222,9 @@
   </si>
   <si>
     <t>WYOMING</t>
+  </si>
+  <si>
+    <t>&lt;3</t>
   </si>
 </sst>
 </file>
@@ -582,486 +543,620 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD50"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A2:A17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" customWidth="1"/>
-    <col min="28" max="28" width="12" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>53</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>28</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>96</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>116</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>56</v>
+      </c>
+      <c r="M4">
+        <v>43</v>
+      </c>
+      <c r="N4">
+        <v>82</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>18</v>
+      </c>
+      <c r="N5">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>781</v>
+      </c>
+      <c r="C6">
+        <v>108</v>
+      </c>
+      <c r="D6">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>979</v>
+      </c>
+      <c r="G6">
+        <v>89</v>
+      </c>
+      <c r="H6">
+        <v>21</v>
+      </c>
+      <c r="I6">
+        <v>79</v>
+      </c>
+      <c r="J6">
+        <v>39</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>527</v>
+      </c>
+      <c r="M6">
+        <v>252</v>
+      </c>
+      <c r="N6">
+        <v>729</v>
+      </c>
+      <c r="O6">
+        <v>31</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>53</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
+      <c r="K15">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L15">
+        <v>22</v>
+      </c>
+      <c r="M15">
+        <v>11</v>
+      </c>
+      <c r="N15">
+        <v>31</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" t="s">
-        <v>15</v>
-      </c>
-      <c r="X1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B14">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.245</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1">
-        <v>9.4E-2</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" s="1">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="J14">
-        <v>53</v>
-      </c>
-      <c r="K14">
-        <v>12</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="M14">
-        <v>3</v>
-      </c>
-      <c r="N14" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>7</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="Q14">
-        <v>6</v>
-      </c>
-      <c r="R14" s="1">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="S14">
-        <v>10</v>
-      </c>
-      <c r="T14" s="1">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="U14">
-        <v>22</v>
-      </c>
-      <c r="V14" s="1">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="W14">
-        <v>11</v>
-      </c>
-      <c r="X14" s="1">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="Y14">
-        <v>31</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>0.96899999999999997</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>16</v>
-      </c>
-      <c r="AD14" s="1">
-        <v>0.40600000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>